<commit_message>
FINFLUX-2815  Stabilaizing automation script
</commit_message>
<xml_diff>
--- a/Finflux Automation Excels/Client/2475-RBI-EI-DB-SAR-REC-NOCOM-RNI-CTPD-DL-MD-TR-2-DATE-VAR-INST-PERIODIC-Makerepayment2.xlsx
+++ b/Finflux Automation Excels/Client/2475-RBI-EI-DB-SAR-REC-NOCOM-RNI-CTPD-DL-MD-TR-2-DATE-VAR-INST-PERIODIC-Makerepayment2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mifosx-e2e-testing\Mifos Automation Excels\Client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\finflux_automation_test\Finflux Automation Excels\Client\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="5" r:id="rId1"/>
@@ -219,7 +219,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,11 +320,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -333,9 +338,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -358,6 +360,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,18 +730,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>42064</v>
       </c>
     </row>
@@ -740,13 +761,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -770,80 +791,80 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="6">
         <v>10000</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="7">
         <v>1681.05</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="9">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
         <v>8318.9500000000007</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>555.6</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <v>95.93</v>
       </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
         <v>459.67</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="A4" s="4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>0</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="A5" s="4">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
         <v>0</v>
       </c>
     </row>
@@ -856,667 +877,668 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="21" customWidth="1"/>
-    <col min="15" max="15" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="4.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="13.85546875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="N1" s="20"/>
+      <c r="O1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24">
         <v>42005</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="8">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="25">
         <v>5000</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6">
-        <v>0</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="Q2" s="6"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23">
+        <v>0</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23">
+        <v>0</v>
+      </c>
+      <c r="L2" s="23">
+        <v>0</v>
+      </c>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="Q2" s="23"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="23">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="23">
         <v>45</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="24">
         <v>42050</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="24">
         <v>42050</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="6">
+      <c r="E3" s="26"/>
+      <c r="F3" s="23">
         <v>813.49</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="27">
         <v>4186.51</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="23">
         <v>75</v>
       </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6">
+      <c r="I3" s="23">
+        <v>0</v>
+      </c>
+      <c r="J3" s="23">
+        <v>0</v>
+      </c>
+      <c r="K3" s="23">
         <v>888.49</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="23">
         <v>888.49</v>
       </c>
-      <c r="M3" s="6">
-        <v>0</v>
-      </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="6">
+      <c r="M3" s="23">
+        <v>0</v>
+      </c>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>42064</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="8">
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="25">
         <v>5000</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="Q4" s="6"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23">
+        <v>0</v>
+      </c>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23">
+        <v>0</v>
+      </c>
+      <c r="L4" s="23">
+        <v>0</v>
+      </c>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="Q4" s="23"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="23">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="23">
         <v>14</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="24">
         <v>42064</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="24">
         <v>42064</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="6">
+      <c r="E5" s="26"/>
+      <c r="F5" s="23">
         <v>867.56</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="27">
         <v>8318.9500000000007</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="23">
         <v>20.93</v>
       </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
+      <c r="I5" s="23">
+        <v>0</v>
+      </c>
+      <c r="J5" s="23">
+        <v>0</v>
+      </c>
+      <c r="K5" s="23">
         <v>888.49</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="23">
         <v>888.49</v>
       </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6">
+      <c r="M5" s="23">
+        <v>0</v>
+      </c>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="23">
         <v>3</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="23">
         <v>31</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="24">
         <v>42095</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23">
         <v>805.3</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="27">
         <v>7513.65</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="23">
         <v>83.19</v>
       </c>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
+      <c r="I6" s="23">
+        <v>0</v>
+      </c>
+      <c r="J6" s="23">
+        <v>0</v>
+      </c>
+      <c r="K6" s="23">
         <v>888.49</v>
       </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="6">
+      <c r="L6" s="23">
+        <v>0</v>
+      </c>
+      <c r="M6" s="23">
+        <v>0</v>
+      </c>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="23">
         <v>888.49</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="23">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="23">
         <v>30</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="24">
         <v>42125</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23">
         <v>813.35</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="27">
         <v>6700.3</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="23">
         <v>75.14</v>
       </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0</v>
-      </c>
-      <c r="K7" s="6">
+      <c r="I7" s="23">
+        <v>0</v>
+      </c>
+      <c r="J7" s="23">
+        <v>0</v>
+      </c>
+      <c r="K7" s="23">
         <v>888.49</v>
       </c>
-      <c r="L7" s="6">
-        <v>0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0</v>
-      </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="6">
+      <c r="L7" s="23">
+        <v>0</v>
+      </c>
+      <c r="M7" s="23">
+        <v>0</v>
+      </c>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="23">
         <v>888.49</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="23">
         <v>5</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="23">
         <v>31</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="24">
         <v>42156</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6">
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23">
         <v>821.49</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="27">
         <v>5878.81</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="23">
         <v>67</v>
       </c>
-      <c r="I8" s="6">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
+      <c r="I8" s="23">
+        <v>0</v>
+      </c>
+      <c r="J8" s="23">
+        <v>0</v>
+      </c>
+      <c r="K8" s="23">
         <v>888.49</v>
       </c>
-      <c r="L8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="6">
-        <v>0</v>
-      </c>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="6">
+      <c r="L8" s="23">
+        <v>0</v>
+      </c>
+      <c r="M8" s="23">
+        <v>0</v>
+      </c>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="23">
         <v>888.49</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="23">
         <v>6</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="23">
         <v>30</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="24">
         <v>42186</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6">
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23">
         <v>829.7</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="27">
         <v>5049.1099999999997</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="23">
         <v>58.79</v>
       </c>
-      <c r="I9" s="6">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
+      <c r="I9" s="23">
+        <v>0</v>
+      </c>
+      <c r="J9" s="23">
+        <v>0</v>
+      </c>
+      <c r="K9" s="23">
         <v>888.49</v>
       </c>
-      <c r="L9" s="6">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0</v>
-      </c>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="6">
+      <c r="L9" s="23">
+        <v>0</v>
+      </c>
+      <c r="M9" s="23">
+        <v>0</v>
+      </c>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="23">
         <v>888.49</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="23">
         <v>7</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="23">
         <v>31</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="24">
         <v>42217</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23">
         <v>838</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="27">
         <v>4211.1099999999997</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="23">
         <v>50.49</v>
       </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
+      <c r="I10" s="23">
+        <v>0</v>
+      </c>
+      <c r="J10" s="23">
+        <v>0</v>
+      </c>
+      <c r="K10" s="23">
         <v>888.49</v>
       </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6">
-        <v>0</v>
-      </c>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="6">
+      <c r="L10" s="23">
+        <v>0</v>
+      </c>
+      <c r="M10" s="23">
+        <v>0</v>
+      </c>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="23">
         <v>888.49</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="23">
         <v>8</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="23">
         <v>31</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="24">
         <v>42248</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23">
         <v>846.38</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="27">
         <v>3364.73</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="23">
         <v>42.11</v>
       </c>
-      <c r="I11" s="6">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="6">
+      <c r="I11" s="23">
+        <v>0</v>
+      </c>
+      <c r="J11" s="23">
+        <v>0</v>
+      </c>
+      <c r="K11" s="23">
         <v>888.49</v>
       </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
-        <v>0</v>
-      </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="6">
+      <c r="L11" s="23">
+        <v>0</v>
+      </c>
+      <c r="M11" s="23">
+        <v>0</v>
+      </c>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="23">
         <v>888.49</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="23">
         <v>9</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="23">
         <v>30</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="24">
         <v>42278</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6">
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23">
         <v>854.84</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="27">
         <v>2509.89</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="23">
         <v>33.65</v>
       </c>
-      <c r="I12" s="6">
-        <v>0</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0</v>
-      </c>
-      <c r="K12" s="6">
+      <c r="I12" s="23">
+        <v>0</v>
+      </c>
+      <c r="J12" s="23">
+        <v>0</v>
+      </c>
+      <c r="K12" s="23">
         <v>888.49</v>
       </c>
-      <c r="L12" s="6">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
-        <v>0</v>
-      </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="6">
+      <c r="L12" s="23">
+        <v>0</v>
+      </c>
+      <c r="M12" s="23">
+        <v>0</v>
+      </c>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="23">
         <v>888.49</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="23">
         <v>10</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="23">
         <v>31</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="24">
         <v>42309</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6">
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23">
         <v>863.39</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="27">
         <v>1646.5</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="23">
         <v>25.1</v>
       </c>
-      <c r="I13" s="6">
-        <v>0</v>
-      </c>
-      <c r="J13" s="6">
-        <v>0</v>
-      </c>
-      <c r="K13" s="6">
+      <c r="I13" s="23">
+        <v>0</v>
+      </c>
+      <c r="J13" s="23">
+        <v>0</v>
+      </c>
+      <c r="K13" s="23">
         <v>888.49</v>
       </c>
-      <c r="L13" s="6">
-        <v>0</v>
-      </c>
-      <c r="M13" s="6">
-        <v>0</v>
-      </c>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="6">
+      <c r="L13" s="23">
+        <v>0</v>
+      </c>
+      <c r="M13" s="23">
+        <v>0</v>
+      </c>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="23">
         <v>888.49</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="23">
         <v>11</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="23">
         <v>30</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="24">
         <v>42339</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23">
         <v>872.03</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="23">
         <v>774.47</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="23">
         <v>16.46</v>
       </c>
-      <c r="I14" s="6">
-        <v>0</v>
-      </c>
-      <c r="J14" s="6">
-        <v>0</v>
-      </c>
-      <c r="K14" s="6">
+      <c r="I14" s="23">
+        <v>0</v>
+      </c>
+      <c r="J14" s="23">
+        <v>0</v>
+      </c>
+      <c r="K14" s="23">
         <v>888.49</v>
       </c>
-      <c r="L14" s="6">
-        <v>0</v>
-      </c>
-      <c r="M14" s="6">
-        <v>0</v>
-      </c>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="6">
+      <c r="L14" s="23">
+        <v>0</v>
+      </c>
+      <c r="M14" s="23">
+        <v>0</v>
+      </c>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="23">
         <v>888.49</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="23">
         <v>12</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="23">
         <v>31</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="24">
         <v>42370</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23">
         <v>774.47</v>
       </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
+      <c r="G15" s="23">
+        <v>0</v>
+      </c>
+      <c r="H15" s="23">
         <v>7.74</v>
       </c>
-      <c r="I15" s="6">
-        <v>0</v>
-      </c>
-      <c r="J15" s="6">
-        <v>0</v>
-      </c>
-      <c r="K15" s="6">
+      <c r="I15" s="23">
+        <v>0</v>
+      </c>
+      <c r="J15" s="23">
+        <v>0</v>
+      </c>
+      <c r="K15" s="23">
         <v>782.21</v>
       </c>
-      <c r="L15" s="6">
-        <v>0</v>
-      </c>
-      <c r="M15" s="6">
-        <v>0</v>
-      </c>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="6">
+      <c r="L15" s="23">
+        <v>0</v>
+      </c>
+      <c r="M15" s="23">
+        <v>0</v>
+      </c>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="23">
         <v>782.21</v>
       </c>
     </row>
@@ -1536,17 +1558,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1582,226 +1604,226 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>73</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <v>42095</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="4">
         <v>83.19</v>
       </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
         <v>83.19</v>
       </c>
-      <c r="H2" s="6">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6">
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>72</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>42064</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>888.49</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>867.56</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <v>20.93</v>
       </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="9">
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
         <v>8318.9500000000007</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>70</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>42064</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>20.93</v>
       </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
         <v>20.93</v>
       </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6">
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>68</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>42064</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <v>5000</v>
       </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="9">
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
         <v>9186.51</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>69</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>42050</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>75</v>
       </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
         <v>75</v>
       </c>
-      <c r="H6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>67</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>42050</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>888.49</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <v>813.49</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <v>75</v>
       </c>
-      <c r="H7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-      <c r="J7" s="9">
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
         <v>4186.51</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>66</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>42005</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="6">
         <v>5000</v>
       </c>
-      <c r="F8" s="6">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0</v>
-      </c>
-      <c r="J8" s="8">
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
         <v>5000</v>
       </c>
     </row>
@@ -1860,56 +1882,56 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="10">
         <v>151</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="9">
         <v>42005</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="13"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="10">
         <v>154</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>42005</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13" t="s">
+      <c r="H3" s="10"/>
+      <c r="I3" s="10" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1968,85 +1990,85 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>125</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <v>42050</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>126</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>42050</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19" t="s">
+      <c r="H3" s="16"/>
+      <c r="I3" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>127</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>42050</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="19"/>
+      <c r="I4" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2104,56 +2126,56 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>34</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <v>42064</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="18"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>35</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>42064</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18" t="s">
+      <c r="H3" s="15"/>
+      <c r="I3" s="15" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2172,16 +2194,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="1" width="8" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2214,85 +2236,85 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
+      <c r="A2" s="13">
         <v>138</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="14">
         <v>42064</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="A3" s="13">
         <v>139</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="14">
         <v>42064</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20" t="s">
+      <c r="H3" s="17"/>
+      <c r="I3" s="17" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="A4" s="13">
         <v>140</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="14">
         <v>42064</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="20"/>
+      <c r="I4" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2303,219 +2325,233 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="7.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>130</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <v>42050</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="21"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>131</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>42050</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>132</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>42064</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="21"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>133</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>42064</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21" t="s">
+      <c r="H6" s="18"/>
+      <c r="I6" s="18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>141</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>42095</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="21"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>142</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>42095</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21" t="s">
+      <c r="H9" s="18"/>
+      <c r="I9" s="18" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>